<commit_message>
Fix casos 20200417 Chubut to Buenos Aires
</commit_message>
<xml_diff>
--- a/data/casos.xlsx
+++ b/data/casos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="reporte_vespertino" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2462" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2464" uniqueCount="77">
   <si>
     <t xml:space="preserve">fecha</t>
   </si>
@@ -357,8 +357,8 @@
   </sheetPr>
   <dimension ref="A1:E1151"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1112" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1151" activeCellId="0" sqref="D1151"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1112" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1129" activeCellId="0" sqref="A1129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20425,10 +20425,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20705,6 +20705,23 @@
         <v>0</v>
       </c>
       <c r="E16" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="0" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix caso extra nacion
</commit_message>
<xml_diff>
--- a/data/casos.xlsx
+++ b/data/casos.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2464" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2466" uniqueCount="77">
   <si>
     <t xml:space="preserve">fecha</t>
   </si>
@@ -358,7 +358,7 @@
   <dimension ref="A1:E1151"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1112" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1129" activeCellId="0" sqref="A1129"/>
+      <selection pane="topLeft" activeCell="A1129" activeCellId="1" sqref="A17:E17 A1129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19957,7 +19957,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="A17:E17 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20425,10 +20425,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20722,6 +20722,23 @@
         <v>0</v>
       </c>
       <c r="E17" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -20744,7 +20761,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
+      <selection pane="topLeft" activeCell="A32" activeCellId="1" sqref="A17:E17 A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Update casos recuperados Mendoza
</commit_message>
<xml_diff>
--- a/data/casos.xlsx
+++ b/data/casos.xlsx
@@ -370,7 +370,7 @@
   </sheetPr>
   <dimension ref="A1:E1226"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A246" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
@@ -13505,7 +13505,7 @@
         <v>1</v>
       </c>
       <c r="E772" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="773" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14661,7 +14661,7 @@
         <v>0</v>
       </c>
       <c r="E840" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="841" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15086,7 +15086,7 @@
         <v>0</v>
       </c>
       <c r="E865" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="866" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17211,7 +17211,7 @@
         <v>0</v>
       </c>
       <c r="E990" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="991" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18486,7 +18486,7 @@
         <v>0</v>
       </c>
       <c r="E1065" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1066" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19336,7 +19336,7 @@
         <v>1</v>
       </c>
       <c r="E1115" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21036,7 +21036,7 @@
         <v>0</v>
       </c>
       <c r="E1215" s="0" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="1216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Update 20200421 - incluye Recuperados Cba
</commit_message>
<xml_diff>
--- a/data/casos.xlsx
+++ b/data/casos.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2626" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2680" uniqueCount="81">
   <si>
     <t xml:space="preserve">fecha</t>
   </si>
@@ -262,6 +262,9 @@
     <t xml:space="preserve">2020-04-20</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-04-21</t>
+  </si>
+  <si>
     <t xml:space="preserve">2020-XX-XX</t>
   </si>
 </sst>
@@ -368,9 +371,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1226"/>
+  <dimension ref="A1:E1251"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A246" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
@@ -12859,7 +12862,7 @@
         <v>0</v>
       </c>
       <c r="E734" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="735" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15834,7 +15837,7 @@
         <v>0</v>
       </c>
       <c r="E909" s="0" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="910" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16259,7 +16262,7 @@
         <v>0</v>
       </c>
       <c r="E934" s="0" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
     <row r="935" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16684,7 +16687,7 @@
         <v>0</v>
       </c>
       <c r="E959" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="960" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17109,7 +17112,7 @@
         <v>0</v>
       </c>
       <c r="E984" s="0" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="985" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18384,7 +18387,7 @@
         <v>1</v>
       </c>
       <c r="E1059" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1060" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20067,7 +20070,7 @@
         <v>0</v>
       </c>
       <c r="E1158" s="0" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20492,7 +20495,7 @@
         <v>1</v>
       </c>
       <c r="E1183" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20917,7 +20920,7 @@
         <v>2</v>
       </c>
       <c r="E1208" s="0" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21223,6 +21226,431 @@
         <v>0</v>
       </c>
       <c r="E1226" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1227" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1227" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1227" s="0" t="n">
+        <v>112</v>
+      </c>
+      <c r="D1227" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E1227" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1228" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1228" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1228" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="D1228" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E1228" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1229" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1229" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1229" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="D1229" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E1229" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1230" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1230" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1230" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1230" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1230" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1231" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1231" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1231" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D1231" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1231" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1232" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1232" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1232" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1232" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1232" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1233" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1233" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1233" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1233" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1233" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1234" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1234" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1234" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1234" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1234" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1235" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1235" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1235" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1235" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1235" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1236" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1236" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1236" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1236" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1236" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1237" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1237" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1237" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1237" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1237" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1238" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1238" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1238" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1238" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1238" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1239" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1239" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1239" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1239" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E1239" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1240" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1240" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1240" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1240" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1240" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1241" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1241" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1241" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1241" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1241" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1242" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1242" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1242" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1242" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1242" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1243" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1243" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1243" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="D1243" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1243" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1244" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1244" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1244" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1244" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1244" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1245" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1245" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1245" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1245" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1245" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1246" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1246" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1246" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1246" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1246" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1247" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1247" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1247" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1247" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1247" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1248" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1248" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1248" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1248" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1248" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1249" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1249" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1249" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1249" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1249" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1250" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1250" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1250" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1250" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1250" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1251" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1251" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1251" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1251" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1251" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -21274,7 +21702,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>6</v>
@@ -21291,7 +21719,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>8</v>
@@ -21308,7 +21736,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>7</v>
@@ -21325,7 +21753,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>9</v>
@@ -21342,7 +21770,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>10</v>
@@ -21359,7 +21787,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>11</v>
@@ -21376,7 +21804,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>13</v>
@@ -21393,7 +21821,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>12</v>
@@ -21410,7 +21838,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>14</v>
@@ -21427,7 +21855,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>15</v>
@@ -21444,7 +21872,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>16</v>
@@ -21461,7 +21889,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>17</v>
@@ -21478,7 +21906,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>18</v>
@@ -21495,7 +21923,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>19</v>
@@ -21512,7 +21940,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>20</v>
@@ -21529,7 +21957,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>21</v>
@@ -21546,7 +21974,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>22</v>
@@ -21563,7 +21991,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>23</v>
@@ -21580,7 +22008,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>24</v>
@@ -21597,7 +22025,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>25</v>
@@ -21614,7 +22042,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>26</v>
@@ -21631,7 +22059,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>27</v>
@@ -21648,7 +22076,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>28</v>
@@ -21665,7 +22093,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>29</v>
@@ -21682,7 +22110,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>30</v>
@@ -22046,10 +22474,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A37" activeCellId="1" sqref="1:1 A37"/>
+      <selection pane="topLeft" activeCell="E39" activeCellId="1" sqref="1:1 E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22683,6 +23111,40 @@
         <v>1</v>
       </c>
       <c r="E37" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E39" s="0" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>